<commit_message>
DA 22 | batch 22 | day 1 Completed
</commit_message>
<xml_diff>
--- a/batches/22/week_01_foundations_environment/day_01/day_01.xlsx
+++ b/batches/22/week_01_foundations_environment/day_01/day_01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shira/Documents/work/acciojob/modules/sql/batches/22/week_01_foundations_environment/day_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07AD7F26-B00D-1D49-B894-A4C763634356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81637EE-FBA8-A24E-9FD4-C63F3D561555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{B77C00B8-51C3-F644-B061-77A5D6A6B63D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{B77C00B8-51C3-F644-B061-77A5D6A6B63D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Agenda" sheetId="1" r:id="rId1"/>
+    <sheet name="Software" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,12 +36,269 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="82">
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Store the data</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>manage the data</t>
+  </si>
+  <si>
+    <t>extract the data from different sources</t>
+  </si>
+  <si>
+    <t>it works on relational databases</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Data Visualization</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Deep learning</t>
+  </si>
+  <si>
+    <t>NLP</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>Structured</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Online Shopping App</t>
+  </si>
+  <si>
+    <t>Plateform where sellers and buyers interact</t>
+  </si>
+  <si>
+    <t>Lucknow</t>
+  </si>
+  <si>
+    <t>Banglore</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Keyboard</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Warehouses</t>
+  </si>
+  <si>
+    <t>Storing the products</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Sections</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>You Need to find the location</t>
+  </si>
+  <si>
+    <t>Blueprint</t>
+  </si>
+  <si>
+    <t>Construct the warehouse</t>
+  </si>
+  <si>
+    <t>Cold Storage</t>
+  </si>
+  <si>
+    <t>Normal Storage</t>
+  </si>
+  <si>
+    <t>Parking</t>
+  </si>
+  <si>
+    <t>Power backup</t>
+  </si>
+  <si>
+    <t>Fire Exten..</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Storage Unit</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Servers</t>
+  </si>
+  <si>
+    <t>Cloud Storage</t>
+  </si>
+  <si>
+    <t>DDL</t>
+  </si>
+  <si>
+    <t>Create Alter Drop Delete</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t>Materialised View</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Store Procedure</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Indexes</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Data Objects</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Manufactring</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Catalogue</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Finanace</t>
+  </si>
+  <si>
+    <t>Customer Support</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>DBMS</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Database Engine</t>
+  </si>
+  <si>
+    <t>RDBMS</t>
+  </si>
+  <si>
+    <t>Mysql</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>MS SQL Server</t>
+  </si>
+  <si>
+    <t>Postgres</t>
+  </si>
+  <si>
+    <t>Azure SQL</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Pgadmin4</t>
+  </si>
+  <si>
+    <t>Postgres16</t>
+  </si>
+  <si>
+    <t>VS Code</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,14 +660,450 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F758BA-B364-8A4F-8507-EDEBB24DE742}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A67" zoomScale="237" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>68</v>
+      </c>
+      <c r="D67" t="s">
+        <v>69</v>
+      </c>
+      <c r="E67" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3DC431-5E3D-EA46-AEA8-973BC077EAD0}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="289" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>